<commit_message>
Root and Blind are final
</commit_message>
<xml_diff>
--- a/TestDocs/CrowdControls/Blind.xlsx
+++ b/TestDocs/CrowdControls/Blind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\_Documents\PersonalProjects\league game design\CrowdControls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Projects\LoL_Sandbox\TestDocs\CrowdControls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
   <si>
     <t>Actions</t>
   </si>
@@ -213,6 +213,24 @@
   </si>
   <si>
     <t>BLIND</t>
+  </si>
+  <si>
+    <t>trivial</t>
+  </si>
+  <si>
+    <t>if blinded while auto is in air, its considered a miss. If the debuff times out and an auto is in the air, it still misses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final notes: </t>
+  </si>
+  <si>
+    <t>If the debuff times out and an auto is in the air, it still misses</t>
+  </si>
+  <si>
+    <t>If blinded while auto is in air, its considered a miss</t>
+  </si>
+  <si>
+    <t>Everything else has no differences from the normal behavior</t>
   </si>
 </sst>
 </file>
@@ -636,14 +654,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="1.7109375" customWidth="1"/>
+    <col min="8" max="9" width="1.7109375" customWidth="1"/>
     <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="16" max="16" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -867,7 +886,9 @@
         <v>1</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="9"/>
+      <c r="L11" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -890,7 +911,9 @@
         <v>1</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="9"/>
+      <c r="L12" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -913,7 +936,9 @@
         <v>1</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="9"/>
+      <c r="L13" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -936,7 +961,9 @@
         <v>1</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
@@ -959,7 +986,9 @@
         <v>1</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="9"/>
+      <c r="L15" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
@@ -982,7 +1011,9 @@
         <v>1</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="9"/>
+      <c r="L16" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
@@ -1005,7 +1036,9 @@
         <v>1</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
@@ -1028,7 +1061,9 @@
         <v>1</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="9"/>
+      <c r="L18" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -1093,7 +1128,9 @@
         <v>1</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="9"/>
+      <c r="L21" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
@@ -1116,7 +1153,9 @@
         <v>1</v>
       </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="9"/>
+      <c r="L22" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
@@ -1139,7 +1178,9 @@
         <v>1</v>
       </c>
       <c r="K23" s="1"/>
-      <c r="L23" s="9"/>
+      <c r="L23" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
@@ -1162,7 +1203,9 @@
         <v>1</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="9"/>
+      <c r="L24" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
@@ -1185,7 +1228,9 @@
         <v>1</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="9"/>
+      <c r="L25" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
@@ -1208,7 +1253,9 @@
         <v>1</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="9"/>
+      <c r="L26" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
@@ -1231,7 +1278,9 @@
         <v>1</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" s="9"/>
+      <c r="L27" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
@@ -1254,7 +1303,9 @@
         <v>1</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="9"/>
+      <c r="L28" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
@@ -1319,7 +1370,9 @@
         <v>1</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="L31" s="9"/>
+      <c r="L31" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
@@ -1342,7 +1395,9 @@
         <v>1</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" s="9"/>
+      <c r="L32" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
@@ -1365,7 +1420,9 @@
         <v>1</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="L33" s="9"/>
+      <c r="L33" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
@@ -1388,7 +1445,9 @@
         <v>1</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="9"/>
+      <c r="L34" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
@@ -1411,7 +1470,9 @@
         <v>1</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="9"/>
+      <c r="L35" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
@@ -1434,7 +1495,9 @@
         <v>1</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="9"/>
+      <c r="L36" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
@@ -1457,7 +1520,9 @@
         <v>1</v>
       </c>
       <c r="K37" s="1"/>
-      <c r="L37" s="9"/>
+      <c r="L37" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
@@ -1480,7 +1545,9 @@
         <v>1</v>
       </c>
       <c r="K38" s="1"/>
-      <c r="L38" s="9"/>
+      <c r="L38" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
@@ -1545,7 +1612,9 @@
         <v>1</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="9"/>
+      <c r="L41" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
@@ -1568,7 +1637,9 @@
         <v>1</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" s="9"/>
+      <c r="L42" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
@@ -1591,7 +1662,9 @@
         <v>1</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="9"/>
+      <c r="L43" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
@@ -1614,7 +1687,9 @@
         <v>1</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="9"/>
+      <c r="L44" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
@@ -1637,7 +1712,9 @@
         <v>1</v>
       </c>
       <c r="K45" s="1"/>
-      <c r="L45" s="9"/>
+      <c r="L45" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
@@ -1660,7 +1737,9 @@
         <v>1</v>
       </c>
       <c r="K46" s="1"/>
-      <c r="L46" s="9"/>
+      <c r="L46" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
@@ -1683,7 +1762,9 @@
         <v>1</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="L47" s="9"/>
+      <c r="L47" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
@@ -1706,7 +1787,9 @@
         <v>1</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="L48" s="9"/>
+      <c r="L48" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
@@ -1771,7 +1854,9 @@
         <v>1</v>
       </c>
       <c r="K51" s="1"/>
-      <c r="L51" s="9"/>
+      <c r="L51" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
@@ -1794,7 +1879,9 @@
         <v>1</v>
       </c>
       <c r="K52" s="1"/>
-      <c r="L52" s="9"/>
+      <c r="L52" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
@@ -1817,7 +1904,9 @@
         <v>1</v>
       </c>
       <c r="K53" s="1"/>
-      <c r="L53" s="9"/>
+      <c r="L53" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
@@ -1840,7 +1929,9 @@
         <v>1</v>
       </c>
       <c r="K54" s="1"/>
-      <c r="L54" s="9"/>
+      <c r="L54" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
@@ -1863,7 +1954,9 @@
         <v>1</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="9"/>
+      <c r="L55" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
@@ -1886,7 +1979,9 @@
         <v>1</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="9"/>
+      <c r="L56" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
@@ -1909,7 +2004,9 @@
         <v>1</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="9"/>
+      <c r="L57" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
@@ -1932,7 +2029,9 @@
         <v>1</v>
       </c>
       <c r="K58" s="1"/>
-      <c r="L58" s="9"/>
+      <c r="L58" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
@@ -1997,7 +2096,9 @@
         <v>1</v>
       </c>
       <c r="K61" s="1"/>
-      <c r="L61" s="9"/>
+      <c r="L61" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
@@ -2020,7 +2121,9 @@
         <v>1</v>
       </c>
       <c r="K62" s="1"/>
-      <c r="L62" s="9"/>
+      <c r="L62" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
@@ -2043,7 +2146,9 @@
         <v>1</v>
       </c>
       <c r="K63" s="1"/>
-      <c r="L63" s="9"/>
+      <c r="L63" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
@@ -2066,7 +2171,9 @@
         <v>1</v>
       </c>
       <c r="K64" s="1"/>
-      <c r="L64" s="9"/>
+      <c r="L64" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9"/>
@@ -2089,7 +2196,9 @@
         <v>1</v>
       </c>
       <c r="K65" s="1"/>
-      <c r="L65" s="9"/>
+      <c r="L65" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
       <c r="O65" s="9"/>
@@ -2112,7 +2221,9 @@
         <v>1</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="L66" s="9"/>
+      <c r="L66" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
@@ -2135,7 +2246,9 @@
         <v>1</v>
       </c>
       <c r="K67" s="1"/>
-      <c r="L67" s="9"/>
+      <c r="L67" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
@@ -2158,7 +2271,9 @@
         <v>1</v>
       </c>
       <c r="K68" s="1"/>
-      <c r="L68" s="9"/>
+      <c r="L68" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
       <c r="O68" s="9"/>
@@ -2186,14 +2301,30 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
+      <c r="B70" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
       <c r="Q70" s="8"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
+      <c r="C71" t="s">
+        <v>66</v>
+      </c>
       <c r="Q71" s="8"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
       <c r="Q72" s="8"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -2443,7 +2574,8 @@
       <c r="Q142" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="122">
+  <mergeCells count="123">
+    <mergeCell ref="C70:G70"/>
     <mergeCell ref="B3:P4"/>
     <mergeCell ref="B7:H8"/>
     <mergeCell ref="L7:P8"/>

</xml_diff>